<commit_message>
FK THIS TABLE SRSLY
1
</commit_message>
<xml_diff>
--- a/Classes.xlsx
+++ b/Classes.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="62">
   <si>
     <t>Items</t>
   </si>
@@ -110,9 +110,6 @@
     <t>PosY(int)</t>
   </si>
   <si>
-    <t>Sprite(Sprite)</t>
-  </si>
-  <si>
     <t>Collision(bool)</t>
   </si>
   <si>
@@ -179,10 +176,43 @@
     <t>ID(int)</t>
   </si>
   <si>
-    <t>TriggerID(int)</t>
-  </si>
-  <si>
     <t>Status(bool)</t>
+  </si>
+  <si>
+    <t>ConnectionID(int)</t>
+  </si>
+  <si>
+    <t>NonLive(logical)</t>
+  </si>
+  <si>
+    <t>Aggressive(bool)</t>
+  </si>
+  <si>
+    <t>AgroRange(SDL_Rect)</t>
+  </si>
+  <si>
+    <t>Sprite(SDL_Sprite)</t>
+  </si>
+  <si>
+    <t>Count(int)</t>
+  </si>
+  <si>
+    <t>Defence(int)</t>
+  </si>
+  <si>
+    <t>AD(int)</t>
+  </si>
+  <si>
+    <t>MaxCount(int)</t>
+  </si>
+  <si>
+    <t>Slot</t>
+  </si>
+  <si>
+    <t>EQ_Sprite(SDL_Sprite)</t>
+  </si>
+  <si>
+    <t>RequireItemID(int)</t>
   </si>
 </sst>
 </file>
@@ -310,7 +340,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -334,19 +364,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -357,19 +374,6 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -405,13 +409,16 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -426,13 +433,13 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -441,14 +448,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -734,7 +738,7 @@
   <dimension ref="A1:AF76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -791,24 +795,24 @@
       <c r="AF1" s="2"/>
     </row>
     <row r="2" spans="1:32" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="14" t="s">
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
@@ -829,28 +833,28 @@
       <c r="AF2" s="2"/>
     </row>
     <row r="3" spans="1:32" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16" t="s">
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="21" t="s">
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="19" t="s">
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="19"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+      <c r="N3" s="20"/>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
@@ -871,34 +875,34 @@
       <c r="AF3" s="2"/>
     </row>
     <row r="4" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17" t="s">
+      <c r="B4" s="18"/>
+      <c r="C4" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17" t="s">
+      <c r="D4" s="18"/>
+      <c r="E4" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="17"/>
+      <c r="F4" s="18"/>
       <c r="G4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="12" t="s">
+      <c r="H4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="18" t="s">
+      <c r="I4" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="18"/>
-      <c r="K4" s="20" t="s">
+      <c r="J4" s="19"/>
+      <c r="K4" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="13" t="s">
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="12" t="s">
         <v>20</v>
       </c>
       <c r="O4" s="2"/>
@@ -3417,22 +3421,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="0.28515625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="33.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="3"/>
   </cols>
@@ -3445,167 +3449,207 @@
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
     </row>
     <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="24" t="s">
+    </row>
+    <row r="6" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="2:11" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+    </row>
+    <row r="8" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="C8" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="2:11" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+    </row>
+    <row r="13" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="2:6" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="23"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+    </row>
+    <row r="18" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="2:6" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+    </row>
+    <row r="27" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="2:6" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="23"/>
+    </row>
+    <row r="29" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="2:4" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33" s="24"/>
+      <c r="D33" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="2:4" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C38" s="23"/>
+    </row>
+    <row r="39" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C39" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E3" s="24"/>
-      <c r="F3" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B38" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B39" s="3" t="s">
+    </row>
+    <row r="42" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="2:4" ht="21" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C43" s="23"/>
+    </row>
+    <row r="44" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B43" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B44" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B2:K2"/>
+  <mergeCells count="8">
     <mergeCell ref="B7:J7"/>
     <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B2:I2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3613,12 +3657,127 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B62"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="20.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B42" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3627,7 +3786,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>